<commit_message>
Corrección Escaleta 1 de 10º
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion01/Escaleta_LE_10_01_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion01/Escaleta_LE_10_01_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csepulveda\Desktop\ESCALETAS GUIONES 1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="9980" yWindow="0" windowWidth="25600" windowHeight="13340"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="320">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1120,12 +1115,78 @@
   <si>
     <t>(DBA: 4, 13, 14) Recurso elaborado por el autor. Aprobado para digitalizar. Obervar que la descripción se modifica un poco. A su vez, dar más claridad en el Enunciado Principal (Instrucción), que se entienda cómo va a desarrollarse la parte de la exposición a la clase.</t>
   </si>
+  <si>
+    <t xml:space="preserve">LE_10_01_COEl análisis literario Lingüística: el signo lingüístico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: las características del signo lingüístico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para comprender las características del signo lingüístico </t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lectura crítica: el análisis de textos literariosConsolidación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: titular párrafos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para desarrollar habilidades lectoras </t>
+  </si>
+  <si>
+    <t>Proponer ejercicio para aplicar la estrategia de titular párrafos. Se les pueden dar los párrafos y también ponerlos a reflexionar sobre esta estrategia, que digan por qué es útil, cuándo la emplearían…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RM </t>
+  </si>
+  <si>
+    <t>Recursos M101A-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producción escrita: el análisis de textos literarios  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: El análisis literario </t>
+  </si>
+  <si>
+    <t>Actividad para aplicar los conocimientos de la literatura española medieval en un análisis literario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proponer un fragmento de la literatura medieval ESPAÑOLA y elaborar preguntas que apunten al análisis literario. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proponer consultar sobre el signo lingüístico y algunos autores como Saussure y Pierce. Para llegar a conclusiones sobre lo que es el signo lingüístico. Proponer preguntas que busquen analizar lo que dice cada uno. </t>
+  </si>
+  <si>
+    <t>Recursos M101A-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debe incluirse 10 preguntas. 3 de la sección de literatura. 2 de lingüística. 2 de ortografía. 2 de comprensión y 1 de Producción. </t>
+  </si>
+  <si>
+    <t>Recurso M101AP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividades para repasar los contenidos del tema El análisi literario. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE_10_01_CO El análisis literario Banco de actividades </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE_10_01_CO El análisis literario Lingüística: el signo lingüístico </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1182,6 +1243,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1264,7 +1338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1535,8 +1609,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="413">
+  <cellStyleXfs count="415">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1950,8 +2053,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2055,6 +2160,70 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2077,7 +2246,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="413">
+  <cellStyles count="415">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -2284,6 +2453,7 @@
     <cellStyle name="Hipervínculo" xfId="407" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="409" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="413" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2490,6 +2660,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="408" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="410" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="414" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2760,7 +2931,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2768,128 +2939,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U91"/>
+  <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
-    <col min="5" max="5" width="58.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.83203125" customWidth="1"/>
+    <col min="5" max="5" width="58.83203125" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="59" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="92.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="92.33203125" customWidth="1"/>
     <col min="11" max="11" width="14" style="9" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" customWidth="1"/>
-    <col min="15" max="15" width="64.28515625" style="10" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" style="7" customWidth="1"/>
-    <col min="17" max="17" width="7.7109375" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" customWidth="1"/>
+    <col min="15" max="15" width="64.33203125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" customWidth="1"/>
+    <col min="18" max="18" width="7.5" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="36.42578125" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="36.5" customWidth="1"/>
+    <col min="21" max="21" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="65" t="s">
+      <c r="H1" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="65" t="s">
+      <c r="J1" s="105" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="65" t="s">
+      <c r="N1" s="107"/>
+      <c r="O1" s="105" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="65" t="s">
+      <c r="P1" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="Q1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="65" t="s">
+      <c r="S1" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="65" t="s">
+      <c r="T1" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="65" t="s">
+      <c r="U1" s="105" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="69"/>
+    <row r="2" spans="1:21" s="12" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109"/>
       <c r="M2" s="17" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>68</v>
       </c>
@@ -2948,7 +3119,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1">
       <c r="A4" s="20" t="s">
         <v>68</v>
       </c>
@@ -3007,7 +3178,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="28">
       <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
@@ -3066,7 +3237,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="56">
       <c r="A6" s="20" t="s">
         <v>68</v>
       </c>
@@ -3125,7 +3296,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="28">
       <c r="A7" s="20" t="s">
         <v>68</v>
       </c>
@@ -3184,7 +3355,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="42">
       <c r="A8" s="20" t="s">
         <v>68</v>
       </c>
@@ -3243,7 +3414,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="28">
       <c r="A9" s="20" t="s">
         <v>68</v>
       </c>
@@ -3302,7 +3473,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="56">
       <c r="A10" s="20" t="s">
         <v>68</v>
       </c>
@@ -3365,7 +3536,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="42">
       <c r="A11" s="20" t="s">
         <v>68</v>
       </c>
@@ -3426,7 +3597,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15" customHeight="1">
       <c r="A12" s="20" t="s">
         <v>68</v>
       </c>
@@ -3487,7 +3658,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15" customHeight="1">
       <c r="A13" s="20" t="s">
         <v>68</v>
       </c>
@@ -3548,7 +3719,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="42">
       <c r="A14" s="20" t="s">
         <v>68</v>
       </c>
@@ -3609,7 +3780,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" s="20" t="s">
         <v>68</v>
       </c>
@@ -3670,7 +3841,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="56">
       <c r="A16" s="20" t="s">
         <v>68</v>
       </c>
@@ -3731,7 +3902,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21">
       <c r="A17" s="20" t="s">
         <v>68</v>
       </c>
@@ -3792,7 +3963,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="28">
       <c r="A18" s="20" t="s">
         <v>68</v>
       </c>
@@ -3853,7 +4024,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="28">
       <c r="A19" s="20" t="s">
         <v>68</v>
       </c>
@@ -3914,7 +4085,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="42">
       <c r="A20" s="20" t="s">
         <v>68</v>
       </c>
@@ -3973,7 +4144,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="28">
       <c r="A21" s="20" t="s">
         <v>68</v>
       </c>
@@ -4034,7 +4205,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21">
       <c r="A22" s="20" t="s">
         <v>68</v>
       </c>
@@ -4093,7 +4264,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="56">
       <c r="A23" s="20" t="s">
         <v>68</v>
       </c>
@@ -4154,7 +4325,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21">
       <c r="A24" s="20" t="s">
         <v>68</v>
       </c>
@@ -4213,7 +4384,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="70">
       <c r="A25" s="20" t="s">
         <v>68</v>
       </c>
@@ -4274,7 +4445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="28">
       <c r="A26" s="20" t="s">
         <v>68</v>
       </c>
@@ -4335,7 +4506,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="28">
       <c r="A27" s="20" t="s">
         <v>68</v>
       </c>
@@ -4394,66 +4565,64 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:21" ht="42">
+      <c r="A28" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H28" s="34">
+      <c r="B28" s="69" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" s="70"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67" t="s">
+        <v>299</v>
+      </c>
+      <c r="H28" s="72">
         <v>26</v>
       </c>
-      <c r="I28" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="J28" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="K28" s="38" t="s">
+      <c r="I28" s="72" t="s">
+        <v>300</v>
+      </c>
+      <c r="J28" s="73" t="s">
+        <v>301</v>
+      </c>
+      <c r="K28" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="L28" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="O28" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="P28" s="40" t="s">
+      <c r="L28" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="M28" s="76" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="42"/>
+      <c r="O28" s="77" t="s">
+        <v>313</v>
+      </c>
+      <c r="P28" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="1">
+      <c r="Q28" s="79">
         <v>6</v>
       </c>
-      <c r="R28" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="S28" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="T28" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="U28" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R28" s="79" t="s">
+        <v>93</v>
+      </c>
+      <c r="S28" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="T28" s="79" t="s">
+        <v>302</v>
+      </c>
+      <c r="U28" s="80" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="42">
       <c r="A29" s="20" t="s">
         <v>68</v>
       </c>
@@ -4469,7 +4638,7 @@
       <c r="E29" s="27"/>
       <c r="F29" s="28"/>
       <c r="G29" s="33" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="H29" s="34">
         <v>27</v>
@@ -4478,39 +4647,41 @@
         <v>92</v>
       </c>
       <c r="J29" s="35" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K29" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L29" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
+      <c r="N29" s="42" t="s">
+        <v>45</v>
+      </c>
       <c r="O29" s="41" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="P29" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="1" t="s">
-        <v>113</v>
+      <c r="Q29" s="1">
+        <v>6</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="S29" s="13" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="T29" s="13" t="s">
-        <v>107</v>
+        <v>189</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" s="20" t="s">
         <v>68</v>
       </c>
@@ -4526,7 +4697,7 @@
       <c r="E30" s="27"/>
       <c r="F30" s="28"/>
       <c r="G30" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H30" s="34">
         <v>28</v>
@@ -4535,7 +4706,7 @@
         <v>92</v>
       </c>
       <c r="J30" s="35" t="s">
-        <v>100</v>
+        <v>192</v>
       </c>
       <c r="K30" s="38" t="s">
         <v>70</v>
@@ -4561,13 +4732,13 @@
         <v>106</v>
       </c>
       <c r="T30" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21">
       <c r="A31" s="20" t="s">
         <v>68</v>
       </c>
@@ -4583,7 +4754,7 @@
       <c r="E31" s="27"/>
       <c r="F31" s="28"/>
       <c r="G31" s="33" t="s">
-        <v>194</v>
+        <v>99</v>
       </c>
       <c r="H31" s="34">
         <v>29</v>
@@ -4592,7 +4763,7 @@
         <v>92</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>196</v>
+        <v>100</v>
       </c>
       <c r="K31" s="38" t="s">
         <v>70</v>
@@ -4618,13 +4789,13 @@
         <v>106</v>
       </c>
       <c r="T31" s="13" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="U31" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21">
       <c r="A32" s="20" t="s">
         <v>68</v>
       </c>
@@ -4637,12 +4808,10 @@
       <c r="D32" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>152</v>
-      </c>
+      <c r="E32" s="27"/>
       <c r="F32" s="28"/>
       <c r="G32" s="33" t="s">
-        <v>257</v>
+        <v>194</v>
       </c>
       <c r="H32" s="34">
         <v>30</v>
@@ -4651,41 +4820,39 @@
         <v>92</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K32" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M32" s="42" t="s">
-        <v>77</v>
-      </c>
+      <c r="M32" s="42"/>
       <c r="N32" s="42"/>
       <c r="O32" s="41" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="P32" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q32" s="1">
-        <v>6</v>
+      <c r="Q32" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="R32" s="13" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="S32" s="13" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="T32" s="13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="28">
       <c r="A33" s="20" t="s">
         <v>68</v>
       </c>
@@ -4703,7 +4870,7 @@
       </c>
       <c r="F33" s="28"/>
       <c r="G33" s="33" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
       <c r="H33" s="34">
         <v>31</v>
@@ -4712,7 +4879,7 @@
         <v>92</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K33" s="38" t="s">
         <v>69</v>
@@ -4721,14 +4888,14 @@
         <v>32</v>
       </c>
       <c r="M33" s="42" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="N33" s="42"/>
       <c r="O33" s="41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P33" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q33" s="1">
         <v>6</v>
@@ -4740,13 +4907,13 @@
         <v>94</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="U33" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="28">
       <c r="A34" s="20" t="s">
         <v>68</v>
       </c>
@@ -4757,55 +4924,57 @@
         <v>91</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>188</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>152</v>
+      </c>
       <c r="F34" s="28"/>
       <c r="G34" s="33" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="H34" s="34">
         <v>32</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="J34" s="35" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K34" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L34" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42" t="s">
-        <v>41</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="M34" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="N34" s="42"/>
       <c r="O34" s="41" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="P34" s="40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q34" s="1">
         <v>6</v>
       </c>
       <c r="R34" s="13" t="s">
-        <v>157</v>
+        <v>93</v>
       </c>
       <c r="S34" s="13" t="s">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="T34" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="U34" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="42">
       <c r="A35" s="20" t="s">
         <v>68</v>
       </c>
@@ -4818,55 +4987,53 @@
       <c r="D35" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="27" t="s">
-        <v>211</v>
-      </c>
+      <c r="E35" s="27"/>
       <c r="F35" s="28"/>
       <c r="G35" s="33" t="s">
-        <v>212</v>
+        <v>91</v>
       </c>
       <c r="H35" s="34">
         <v>33</v>
       </c>
-      <c r="I35" s="31" t="s">
-        <v>92</v>
+      <c r="I35" s="34" t="s">
+        <v>114</v>
       </c>
       <c r="J35" s="35" t="s">
-        <v>213</v>
-      </c>
-      <c r="K35" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="K35" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="L35" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="M35" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42" t="s">
-        <v>285</v>
+      <c r="L35" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="O35" s="41" t="s">
+        <v>284</v>
       </c>
       <c r="P35" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="Q35" s="1">
         <v>6</v>
       </c>
-      <c r="R35" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="S35" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="T35" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="U35" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="R35" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="S35" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="T35" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="28">
       <c r="A36" s="20" t="s">
         <v>68</v>
       </c>
@@ -4880,33 +5047,33 @@
         <v>201</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F36" s="28"/>
       <c r="G36" s="33" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="H36" s="34">
         <v>34</v>
       </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>258</v>
-      </c>
-      <c r="K36" s="38" t="s">
+      <c r="J36" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="K36" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="39" t="s">
+      <c r="L36" s="37" t="s">
         <v>32</v>
       </c>
       <c r="M36" s="42" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N36" s="42"/>
-      <c r="O36" s="41" t="s">
-        <v>286</v>
+      <c r="O36" s="42" t="s">
+        <v>285</v>
       </c>
       <c r="P36" s="40" t="s">
         <v>19</v>
@@ -4921,135 +5088,131 @@
         <v>94</v>
       </c>
       <c r="T36" s="14" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="U36" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="46" t="s">
+    <row r="37" spans="1:21" ht="28">
+      <c r="A37" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="49" t="s">
+      <c r="D37" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E37" s="50" t="s">
+      <c r="E37" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52" t="s">
-        <v>214</v>
-      </c>
-      <c r="H37" s="53">
+      <c r="F37" s="28"/>
+      <c r="G37" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="H37" s="34">
         <v>35</v>
       </c>
-      <c r="I37" s="54" t="s">
+      <c r="I37" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="J37" s="55" t="s">
-        <v>215</v>
-      </c>
-      <c r="K37" s="56" t="s">
+      <c r="J37" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="K37" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="L37" s="57" t="s">
+      <c r="L37" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M37" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58" t="s">
-        <v>290</v>
-      </c>
-      <c r="P37" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q37" s="60">
+      <c r="M37" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="N37" s="42"/>
+      <c r="O37" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="P37" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q37" s="3">
         <v>6</v>
       </c>
-      <c r="R37" s="60" t="s">
+      <c r="R37" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="S37" s="60" t="s">
+      <c r="S37" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="T37" s="60" t="s">
-        <v>225</v>
-      </c>
-      <c r="U37" s="61" t="s">
+      <c r="T37" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="U37" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
+    <row r="38" spans="1:21" ht="42">
+      <c r="A38" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" s="51"/>
-      <c r="G38" s="52" t="s">
-        <v>220</v>
-      </c>
-      <c r="H38" s="53">
+      <c r="B38" s="69" t="s">
+        <v>298</v>
+      </c>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71" t="s">
+        <v>303</v>
+      </c>
+      <c r="E38" s="65"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="67" t="s">
+        <v>304</v>
+      </c>
+      <c r="H38" s="72">
         <v>36</v>
       </c>
-      <c r="I38" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="J38" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="K38" s="56" t="s">
+      <c r="I38" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="J38" s="83" t="s">
+        <v>305</v>
+      </c>
+      <c r="K38" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="O38" s="58" t="s">
-        <v>291</v>
-      </c>
-      <c r="P38" s="59" t="s">
+      <c r="L38" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="M38" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="N38" s="81"/>
+      <c r="O38" s="86" t="s">
+        <v>306</v>
+      </c>
+      <c r="P38" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="Q38" s="87">
         <v>6</v>
       </c>
-      <c r="R38" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="S38" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="T38" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="U38" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="75" x14ac:dyDescent="0.25">
+      <c r="R38" s="88" t="s">
+        <v>307</v>
+      </c>
+      <c r="S38" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="T38" s="88" t="s">
+        <v>308</v>
+      </c>
+      <c r="U38" s="89" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="28">
       <c r="A39" s="46" t="s">
         <v>68</v>
       </c>
@@ -5060,55 +5223,57 @@
         <v>91</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="H39" s="34">
+        <v>201</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="H39" s="53">
         <v>37</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="J39" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="K39" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="L39" s="39" t="s">
+      <c r="J39" s="55" t="s">
+        <v>215</v>
+      </c>
+      <c r="K39" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="41" t="s">
-        <v>292</v>
-      </c>
-      <c r="P39" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="R39" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="S39" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="T39" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="U39" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="M39" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58" t="s">
+        <v>290</v>
+      </c>
+      <c r="P39" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q39" s="60">
+        <v>6</v>
+      </c>
+      <c r="R39" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="S39" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="T39" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="U39" s="61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="28">
       <c r="A40" s="46" t="s">
         <v>68</v>
       </c>
@@ -5121,71 +5286,73 @@
       <c r="D40" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="E40" s="50" t="s">
-        <v>210</v>
-      </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="H40" s="34">
+      <c r="E40" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="51"/>
+      <c r="G40" s="52" t="s">
+        <v>220</v>
+      </c>
+      <c r="H40" s="53">
         <v>38</v>
       </c>
-      <c r="I40" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="J40" s="35" t="s">
-        <v>207</v>
-      </c>
-      <c r="K40" s="36" t="s">
+      <c r="I40" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="J40" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="K40" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="L40" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="M40" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="P40" s="40" t="s">
+      <c r="L40" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="O40" s="58" t="s">
+        <v>291</v>
+      </c>
+      <c r="P40" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q40" s="1">
         <v>6</v>
       </c>
-      <c r="R40" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="S40" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="T40" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="U40" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="R40" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="S40" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="T40" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="56">
+      <c r="A41" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30"/>
+      <c r="D41" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" s="28"/>
       <c r="G41" s="33" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="H41" s="34">
         <v>39</v>
@@ -5194,7 +5361,7 @@
         <v>92</v>
       </c>
       <c r="J41" s="35" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="K41" s="38" t="s">
         <v>70</v>
@@ -5205,7 +5372,7 @@
       <c r="M41" s="42"/>
       <c r="N41" s="42"/>
       <c r="O41" s="41" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="P41" s="40" t="s">
         <v>19</v>
@@ -5220,131 +5387,133 @@
         <v>110</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="U41" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+    <row r="42" spans="1:21" ht="28">
+      <c r="A42" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E42" s="29"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="33" t="s">
-        <v>182</v>
+      <c r="B42" s="92" t="s">
+        <v>298</v>
+      </c>
+      <c r="C42" s="93"/>
+      <c r="D42" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="E42" s="65" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="28"/>
+      <c r="G42" s="67" t="s">
+        <v>310</v>
       </c>
       <c r="H42" s="34">
         <v>40</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="J42" s="35" t="s">
-        <v>183</v>
-      </c>
-      <c r="K42" s="38" t="s">
+      <c r="J42" s="73" t="s">
+        <v>311</v>
+      </c>
+      <c r="K42" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="L42" s="39" t="s">
+      <c r="L42" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="M42" s="42" t="s">
-        <v>61</v>
+      <c r="M42" s="76" t="s">
+        <v>62</v>
       </c>
       <c r="N42" s="42"/>
-      <c r="O42" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="P42" s="40" t="s">
+      <c r="O42" s="76" t="s">
+        <v>312</v>
+      </c>
+      <c r="P42" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="Q42" s="1">
+      <c r="Q42" s="87">
         <v>6</v>
       </c>
-      <c r="R42" s="13" t="s">
+      <c r="R42" s="95" t="s">
         <v>93</v>
       </c>
-      <c r="S42" s="13" t="s">
+      <c r="S42" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="T42" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="U42" s="2" t="s">
+      <c r="T42" s="95" t="s">
+        <v>314</v>
+      </c>
+      <c r="U42" s="96" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+    <row r="43" spans="1:21" ht="42">
+      <c r="A43" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30"/>
+      <c r="D43" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="F43" s="28"/>
       <c r="G43" s="33" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="H43" s="34">
         <v>41</v>
       </c>
-      <c r="I43" s="34" t="s">
+      <c r="I43" s="31" t="s">
         <v>92</v>
       </c>
       <c r="J43" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="K43" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="K43" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="L43" s="39" t="s">
+      <c r="L43" s="37" t="s">
         <v>32</v>
       </c>
       <c r="M43" s="42" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N43" s="42"/>
-      <c r="O43" s="41" t="s">
-        <v>181</v>
+      <c r="O43" s="42" t="s">
+        <v>293</v>
       </c>
       <c r="P43" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q43" s="1">
+      <c r="Q43" s="3">
         <v>6</v>
       </c>
-      <c r="R43" s="13" t="s">
+      <c r="R43" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="S43" s="13" t="s">
+      <c r="S43" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="T43" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="U43" s="2" t="s">
+      <c r="T43" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="U43" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21">
       <c r="A44" s="20" t="s">
         <v>68</v>
       </c>
@@ -5354,13 +5523,13 @@
       <c r="C44" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
       <c r="G44" s="33" t="s">
-        <v>251</v>
+        <v>186</v>
       </c>
       <c r="H44" s="34">
         <v>42</v>
@@ -5369,41 +5538,39 @@
         <v>92</v>
       </c>
       <c r="J44" s="35" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="K44" s="38" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L44" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="42" t="s">
-        <v>64</v>
-      </c>
+      <c r="M44" s="42"/>
       <c r="N44" s="42"/>
       <c r="O44" s="41" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="P44" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q44" s="1">
-        <v>6</v>
+      <c r="Q44" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="R44" s="13" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="S44" s="13" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="T44" s="13" t="s">
-        <v>250</v>
+        <v>185</v>
       </c>
       <c r="U44" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" s="5" customFormat="1">
       <c r="A45" s="20" t="s">
         <v>68</v>
       </c>
@@ -5414,12 +5581,12 @@
         <v>91</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="E45" s="29"/>
       <c r="F45" s="30"/>
       <c r="G45" s="33" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="H45" s="34">
         <v>43</v>
@@ -5428,27 +5595,41 @@
         <v>92</v>
       </c>
       <c r="J45" s="35" t="s">
-        <v>249</v>
+        <v>183</v>
       </c>
       <c r="K45" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L45" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="42"/>
+        <v>32</v>
+      </c>
+      <c r="M45" s="42" t="s">
+        <v>61</v>
+      </c>
       <c r="N45" s="42"/>
-      <c r="O45" s="41"/>
+      <c r="O45" s="41" t="s">
+        <v>295</v>
+      </c>
       <c r="P45" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="13"/>
-      <c r="S45" s="13"/>
-      <c r="T45" s="13"/>
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q45" s="1">
+        <v>6</v>
+      </c>
+      <c r="R45" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="S45" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="T45" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" s="20" t="s">
         <v>68</v>
       </c>
@@ -5459,12 +5640,12 @@
         <v>91</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="E46" s="29"/>
       <c r="F46" s="30"/>
       <c r="G46" s="33" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="H46" s="34">
         <v>44</v>
@@ -5473,7 +5654,7 @@
         <v>92</v>
       </c>
       <c r="J46" s="35" t="s">
-        <v>248</v>
+        <v>180</v>
       </c>
       <c r="K46" s="38" t="s">
         <v>69</v>
@@ -5482,11 +5663,11 @@
         <v>32</v>
       </c>
       <c r="M46" s="42" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="N46" s="42"/>
       <c r="O46" s="41" t="s">
-        <v>221</v>
+        <v>181</v>
       </c>
       <c r="P46" s="40" t="s">
         <v>19</v>
@@ -5501,67 +5682,223 @@
         <v>94</v>
       </c>
       <c r="T46" s="13" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
       <c r="U46" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="24"/>
+    <row r="47" spans="1:21" ht="28">
+      <c r="A47" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" s="27"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="H47" s="34">
+        <v>45</v>
+      </c>
+      <c r="I47" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="J47" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="K47" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L47" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="N47" s="42"/>
+      <c r="O47" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="P47" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>6</v>
+      </c>
+      <c r="R47" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="S47" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>203</v>
+      </c>
       <c r="E48" s="29"/>
       <c r="F48" s="30"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="35"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="39"/>
+      <c r="G48" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="H48" s="34">
+        <v>46</v>
+      </c>
+      <c r="I48" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="J48" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="K48" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48" s="39" t="s">
+        <v>33</v>
+      </c>
       <c r="M48" s="42"/>
       <c r="N48" s="42"/>
       <c r="O48" s="41"/>
-      <c r="P48" s="40"/>
+      <c r="P48" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="13"/>
       <c r="S48" s="13"/>
       <c r="T48" s="13"/>
       <c r="U48" s="2"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="42"/>
+    <row r="49" spans="1:21">
+      <c r="A49" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="E49" s="29"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="H49" s="34">
+        <v>47</v>
+      </c>
+      <c r="I49" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="J49" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="K49" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L49" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M49" s="42" t="s">
+        <v>23</v>
+      </c>
       <c r="N49" s="42"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="40"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="4"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="48"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="30"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O49" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="P49" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>6</v>
+      </c>
+      <c r="R49" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="S49" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="T49" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="28">
+      <c r="A50" s="97" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="98" t="s">
+        <v>318</v>
+      </c>
+      <c r="C50" s="99"/>
+      <c r="D50" s="99"/>
+      <c r="H50" s="7">
+        <v>48</v>
+      </c>
+      <c r="J50" s="73" t="s">
+        <v>317</v>
+      </c>
+      <c r="K50" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="L50" s="101" t="s">
+        <v>32</v>
+      </c>
+      <c r="M50" s="102" t="s">
+        <v>63</v>
+      </c>
+      <c r="N50" s="99"/>
+      <c r="O50" s="103" t="s">
+        <v>315</v>
+      </c>
+      <c r="P50" s="104" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q50" s="99">
+        <v>6</v>
+      </c>
+      <c r="R50" s="99" t="s">
+        <v>93</v>
+      </c>
+      <c r="S50" s="99" t="s">
+        <v>94</v>
+      </c>
+      <c r="T50" s="99" t="s">
+        <v>316</v>
+      </c>
+      <c r="U50" s="99" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" s="20"/>
       <c r="B51" s="21"/>
       <c r="C51" s="22"/>
@@ -5584,53 +5921,38 @@
       <c r="T51" s="13"/>
       <c r="U51" s="2"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21">
       <c r="A52" s="20"/>
       <c r="B52" s="21"/>
       <c r="C52" s="22"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="30"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="33"/>
       <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
+      <c r="I52" s="31"/>
       <c r="J52" s="35"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="39"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="37"/>
       <c r="M52" s="42"/>
       <c r="N52" s="42"/>
-      <c r="O52" s="41"/>
+      <c r="O52" s="42"/>
       <c r="P52" s="40"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="13"/>
-      <c r="S52" s="13"/>
-      <c r="T52" s="13"/>
-      <c r="U52" s="2"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="24"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="4"/>
+    </row>
+    <row r="53" spans="1:21">
+      <c r="A53" s="46"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="23"/>
       <c r="E53" s="29"/>
       <c r="F53" s="30"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="38"/>
-      <c r="L53" s="39"/>
-      <c r="M53" s="42"/>
-      <c r="N53" s="42"/>
-      <c r="O53" s="41"/>
-      <c r="P53" s="40"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="13"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="2"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54" s="20"/>
       <c r="B54" s="21"/>
       <c r="C54" s="22"/>
@@ -5653,7 +5975,7 @@
       <c r="T54" s="13"/>
       <c r="U54" s="2"/>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21">
       <c r="A55" s="20"/>
       <c r="B55" s="21"/>
       <c r="C55" s="22"/>
@@ -5676,7 +5998,7 @@
       <c r="T55" s="13"/>
       <c r="U55" s="2"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21">
       <c r="A56" s="20"/>
       <c r="B56" s="21"/>
       <c r="C56" s="22"/>
@@ -5699,7 +6021,7 @@
       <c r="T56" s="13"/>
       <c r="U56" s="2"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21">
       <c r="A57" s="20"/>
       <c r="B57" s="21"/>
       <c r="C57" s="22"/>
@@ -5722,7 +6044,7 @@
       <c r="T57" s="13"/>
       <c r="U57" s="2"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21">
       <c r="A58" s="20"/>
       <c r="B58" s="21"/>
       <c r="C58" s="22"/>
@@ -5745,7 +6067,7 @@
       <c r="T58" s="13"/>
       <c r="U58" s="2"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21">
       <c r="A59" s="20"/>
       <c r="B59" s="21"/>
       <c r="C59" s="22"/>
@@ -5768,7 +6090,7 @@
       <c r="T59" s="13"/>
       <c r="U59" s="2"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21">
       <c r="A60" s="20"/>
       <c r="B60" s="21"/>
       <c r="C60" s="22"/>
@@ -5791,7 +6113,7 @@
       <c r="T60" s="13"/>
       <c r="U60" s="2"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21">
       <c r="A61" s="20"/>
       <c r="B61" s="21"/>
       <c r="C61" s="22"/>
@@ -5814,7 +6136,7 @@
       <c r="T61" s="13"/>
       <c r="U61" s="2"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21">
       <c r="A62" s="20"/>
       <c r="B62" s="21"/>
       <c r="C62" s="22"/>
@@ -5837,7 +6159,7 @@
       <c r="T62" s="13"/>
       <c r="U62" s="2"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21">
       <c r="A63" s="20"/>
       <c r="B63" s="21"/>
       <c r="C63" s="22"/>
@@ -5860,7 +6182,7 @@
       <c r="T63" s="13"/>
       <c r="U63" s="2"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21">
       <c r="A64" s="20"/>
       <c r="B64" s="21"/>
       <c r="C64" s="22"/>
@@ -5883,7 +6205,7 @@
       <c r="T64" s="13"/>
       <c r="U64" s="2"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21">
       <c r="A65" s="20"/>
       <c r="B65" s="21"/>
       <c r="C65" s="22"/>
@@ -5906,7 +6228,7 @@
       <c r="T65" s="13"/>
       <c r="U65" s="2"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21">
       <c r="A66" s="20"/>
       <c r="B66" s="21"/>
       <c r="C66" s="22"/>
@@ -5929,7 +6251,7 @@
       <c r="T66" s="13"/>
       <c r="U66" s="2"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21">
       <c r="A67" s="20"/>
       <c r="B67" s="21"/>
       <c r="C67" s="22"/>
@@ -5952,7 +6274,7 @@
       <c r="T67" s="13"/>
       <c r="U67" s="2"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21">
       <c r="A68" s="20"/>
       <c r="B68" s="21"/>
       <c r="C68" s="22"/>
@@ -5975,7 +6297,7 @@
       <c r="T68" s="13"/>
       <c r="U68" s="2"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21">
       <c r="A69" s="20"/>
       <c r="B69" s="21"/>
       <c r="C69" s="22"/>
@@ -5998,7 +6320,7 @@
       <c r="T69" s="13"/>
       <c r="U69" s="2"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21">
       <c r="A70" s="20"/>
       <c r="B70" s="21"/>
       <c r="C70" s="22"/>
@@ -6021,7 +6343,7 @@
       <c r="T70" s="13"/>
       <c r="U70" s="2"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21">
       <c r="A71" s="20"/>
       <c r="B71" s="21"/>
       <c r="C71" s="22"/>
@@ -6044,7 +6366,7 @@
       <c r="T71" s="13"/>
       <c r="U71" s="2"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21">
       <c r="A72" s="20"/>
       <c r="B72" s="21"/>
       <c r="C72" s="22"/>
@@ -6067,7 +6389,7 @@
       <c r="T72" s="13"/>
       <c r="U72" s="2"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21">
       <c r="A73" s="20"/>
       <c r="B73" s="21"/>
       <c r="C73" s="22"/>
@@ -6090,7 +6412,7 @@
       <c r="T73" s="13"/>
       <c r="U73" s="2"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21">
       <c r="A74" s="20"/>
       <c r="B74" s="21"/>
       <c r="C74" s="22"/>
@@ -6113,7 +6435,7 @@
       <c r="T74" s="13"/>
       <c r="U74" s="2"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21">
       <c r="A75" s="20"/>
       <c r="B75" s="21"/>
       <c r="C75" s="22"/>
@@ -6136,7 +6458,7 @@
       <c r="T75" s="13"/>
       <c r="U75" s="2"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21">
       <c r="A76" s="20"/>
       <c r="B76" s="21"/>
       <c r="C76" s="22"/>
@@ -6159,7 +6481,7 @@
       <c r="T76" s="13"/>
       <c r="U76" s="2"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21">
       <c r="A77" s="20"/>
       <c r="B77" s="21"/>
       <c r="C77" s="22"/>
@@ -6182,7 +6504,7 @@
       <c r="T77" s="13"/>
       <c r="U77" s="2"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21">
       <c r="A78" s="20"/>
       <c r="B78" s="21"/>
       <c r="C78" s="22"/>
@@ -6205,7 +6527,7 @@
       <c r="T78" s="13"/>
       <c r="U78" s="2"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21">
       <c r="A79" s="20"/>
       <c r="B79" s="21"/>
       <c r="C79" s="22"/>
@@ -6228,7 +6550,7 @@
       <c r="T79" s="13"/>
       <c r="U79" s="2"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21">
       <c r="A80" s="20"/>
       <c r="B80" s="21"/>
       <c r="C80" s="22"/>
@@ -6251,7 +6573,7 @@
       <c r="T80" s="13"/>
       <c r="U80" s="2"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21">
       <c r="A81" s="20"/>
       <c r="B81" s="21"/>
       <c r="C81" s="22"/>
@@ -6274,7 +6596,7 @@
       <c r="T81" s="13"/>
       <c r="U81" s="2"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21">
       <c r="A82" s="20"/>
       <c r="B82" s="21"/>
       <c r="C82" s="22"/>
@@ -6297,7 +6619,7 @@
       <c r="T82" s="13"/>
       <c r="U82" s="2"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21">
       <c r="A83" s="20"/>
       <c r="B83" s="21"/>
       <c r="C83" s="22"/>
@@ -6320,7 +6642,7 @@
       <c r="T83" s="13"/>
       <c r="U83" s="2"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21">
       <c r="A84" s="20"/>
       <c r="B84" s="21"/>
       <c r="C84" s="22"/>
@@ -6343,7 +6665,7 @@
       <c r="T84" s="13"/>
       <c r="U84" s="2"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21">
       <c r="A85" s="20"/>
       <c r="B85" s="21"/>
       <c r="C85" s="22"/>
@@ -6366,7 +6688,7 @@
       <c r="T85" s="13"/>
       <c r="U85" s="2"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21">
       <c r="A86" s="20"/>
       <c r="B86" s="21"/>
       <c r="C86" s="22"/>
@@ -6389,7 +6711,7 @@
       <c r="T86" s="13"/>
       <c r="U86" s="2"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21">
       <c r="A87" s="20"/>
       <c r="B87" s="21"/>
       <c r="C87" s="22"/>
@@ -6412,7 +6734,7 @@
       <c r="T87" s="13"/>
       <c r="U87" s="2"/>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21">
       <c r="A88" s="20"/>
       <c r="B88" s="21"/>
       <c r="C88" s="22"/>
@@ -6435,7 +6757,7 @@
       <c r="T88" s="13"/>
       <c r="U88" s="2"/>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21">
       <c r="A89" s="20"/>
       <c r="B89" s="21"/>
       <c r="C89" s="22"/>
@@ -6458,7 +6780,7 @@
       <c r="T89" s="13"/>
       <c r="U89" s="2"/>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21">
       <c r="A90" s="20"/>
       <c r="B90" s="21"/>
       <c r="C90" s="22"/>
@@ -6481,7 +6803,7 @@
       <c r="T90" s="13"/>
       <c r="U90" s="2"/>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21">
       <c r="A91" s="20"/>
       <c r="B91" s="21"/>
       <c r="C91" s="22"/>
@@ -6504,13 +6826,77 @@
       <c r="T91" s="13"/>
       <c r="U91" s="2"/>
     </row>
+    <row r="92" spans="1:21">
+      <c r="A92" s="20"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="33"/>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="35"/>
+      <c r="K92" s="38"/>
+      <c r="L92" s="39"/>
+      <c r="M92" s="42"/>
+      <c r="N92" s="42"/>
+      <c r="O92" s="41"/>
+      <c r="P92" s="40"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="13"/>
+      <c r="S92" s="13"/>
+      <c r="T92" s="13"/>
+      <c r="U92" s="2"/>
+    </row>
+    <row r="93" spans="1:21">
+      <c r="A93" s="20"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="34"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="35"/>
+      <c r="K93" s="38"/>
+      <c r="L93" s="39"/>
+      <c r="M93" s="42"/>
+      <c r="N93" s="42"/>
+      <c r="O93" s="41"/>
+      <c r="P93" s="40"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="13"/>
+      <c r="S93" s="13"/>
+      <c r="T93" s="13"/>
+      <c r="U93" s="2"/>
+    </row>
+    <row r="94" spans="1:21">
+      <c r="A94" s="20"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="30"/>
+      <c r="G94" s="33"/>
+      <c r="H94" s="34"/>
+      <c r="I94" s="34"/>
+      <c r="J94" s="35"/>
+      <c r="K94" s="38"/>
+      <c r="L94" s="39"/>
+      <c r="M94" s="42"/>
+      <c r="N94" s="42"/>
+      <c r="O94" s="41"/>
+      <c r="P94" s="40"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="13"/>
+      <c r="S94" s="13"/>
+      <c r="T94" s="13"/>
+      <c r="U94" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="M1:N1"/>
@@ -6526,8 +6912,14 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
@@ -6535,37 +6927,37 @@
           <x14:formula1>
             <xm:f>DATOS!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A36 A51:A91 A41:A46 A48:A49</xm:sqref>
+          <xm:sqref>A3:A38 A54:A94 A44:A49 A51:A52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K36 K39:K46 K48:K49 K51:K91</xm:sqref>
+          <xm:sqref>K3:K38 K41:K49 K51:K52 K54:K94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$F$2:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L36 L38:L46 L48:L49 L51:L91</xm:sqref>
+          <xm:sqref>L3:L38 L40:L49 L51:L52 L54:L94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$G$2:$G$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P13:P24 P3:P11 P26:P36 P39:P46 P48:P49 P51:P91</xm:sqref>
+          <xm:sqref>P13:P24 P3:P11 P26:P38 P41:P49 P51:P52 P54:P94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$C$2:$C$39</xm:f>
           </x14:formula1>
-          <xm:sqref>M8:M24 M4 M26:M36 M39:M46 M48:M49 M51:M91</xm:sqref>
+          <xm:sqref>M8:M24 M4 M26:M38 M41:M49 M51:M52 M54:M94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>N9:N24 N4 N26:N36 N39:N46 N48:N49 N51:N91</xm:sqref>
+          <xm:sqref>N9:N24 N4 N26:N38 N41:N49 N51:N52 N54:N94</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6584,16 +6976,16 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -6616,7 +7008,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
         <v>34</v>
@@ -6637,7 +7029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="15"/>
       <c r="B3" s="15" t="s">
         <v>35</v>
@@ -6658,7 +7050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="15"/>
       <c r="B4" s="15" t="s">
         <v>36</v>
@@ -6675,7 +7067,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="15"/>
       <c r="B5" s="15" t="s">
         <v>37</v>
@@ -6692,7 +7084,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="15"/>
       <c r="B6" s="15" t="s">
         <v>38</v>
@@ -6707,7 +7099,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="15"/>
       <c r="B7" s="15" t="s">
         <v>39</v>
@@ -6720,7 +7112,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="15"/>
       <c r="B8" s="15" t="s">
         <v>40</v>
@@ -6733,7 +7125,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="15"/>
       <c r="B9" s="15" t="s">
         <v>41</v>
@@ -6746,7 +7138,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="15"/>
       <c r="B10" s="15" t="s">
         <v>42</v>
@@ -6759,7 +7151,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="15"/>
       <c r="B11" s="15" t="s">
         <v>43</v>
@@ -6774,7 +7166,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="15"/>
       <c r="B12" s="15" t="s">
         <v>44</v>
@@ -6789,7 +7181,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="15"/>
       <c r="B13" s="15" t="s">
         <v>45</v>
@@ -6804,7 +7196,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="15"/>
       <c r="B14" s="15" t="s">
         <v>46</v>
@@ -6819,7 +7211,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
@@ -6832,7 +7224,7 @@
       <c r="M15" s="6"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
@@ -6845,7 +7237,7 @@
       <c r="M16" s="6"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15" t="s">
@@ -6858,7 +7250,7 @@
       <c r="M17" s="6"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
@@ -6871,7 +7263,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
@@ -6884,7 +7276,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
@@ -6897,7 +7289,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
@@ -6910,7 +7302,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
@@ -6923,7 +7315,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15" t="s">
@@ -6936,7 +7328,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
@@ -6949,7 +7341,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
@@ -6960,7 +7352,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
@@ -6971,7 +7363,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
@@ -6982,7 +7374,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15" t="s">
@@ -6993,7 +7385,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
@@ -7004,7 +7396,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15" t="s">
@@ -7015,7 +7407,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
@@ -7026,7 +7418,7 @@
       <c r="F31" s="15"/>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
@@ -7037,7 +7429,7 @@
       <c r="F32" s="15"/>
       <c r="G32" s="11"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
@@ -7048,7 +7440,7 @@
       <c r="F33" s="15"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
@@ -7059,7 +7451,7 @@
       <c r="F34" s="15"/>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15" t="s">
@@ -7070,7 +7462,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
@@ -7081,7 +7473,7 @@
       <c r="F36" s="15"/>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="15" t="s">
@@ -7092,7 +7484,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11" t="s">
@@ -7103,7 +7495,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11" t="s">
@@ -7114,7 +7506,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -7123,7 +7515,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -7132,7 +7524,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -7141,7 +7533,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -7150,7 +7542,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -7159,7 +7551,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -7168,7 +7560,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -7177,7 +7569,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -7186,7 +7578,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -7195,7 +7587,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -7204,7 +7596,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>

</xml_diff>